<commit_message>
modify the matched file
</commit_message>
<xml_diff>
--- a/recordcleaner/CME_matched.xlsx
+++ b/recordcleaner/CME_matched.xlsx
@@ -3147,7 +3147,7 @@
     <t xml:space="preserve">International Index</t>
   </si>
   <si>
-    <t xml:space="preserve">'</t>
+    <t xml:space="preserve"> NIKKEI 225 (YEN) STOCK</t>
   </si>
   <si>
     <t xml:space="preserve"> S&amp;P MATERIALS SECTOR</t>
@@ -4735,7 +4735,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4753,6 +4753,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -18180,8 +18184,8 @@
   </sheetPr>
   <dimension ref="A1:L166"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A89" activeCellId="0" sqref="A89"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18681,7 +18685,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="15" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
         <v>1040</v>
       </c>
@@ -20661,7 +20665,7 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="70" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="s">
         <v>1179</v>
       </c>
@@ -21165,7 +21169,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="84" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="3" t="s">
         <v>1196</v>
       </c>
@@ -21345,7 +21349,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="89" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="3" t="s">
         <v>1210</v>
       </c>
@@ -21647,7 +21651,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
         <v>1231</v>
       </c>
@@ -21676,7 +21680,7 @@
       <c r="J98" s="0" t="s">
         <v>1129</v>
       </c>
-      <c r="K98" s="0" t="s">
+      <c r="K98" s="5" t="s">
         <v>1233</v>
       </c>
       <c r="L98" s="0" t="s">
@@ -21805,183 +21809,183 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="103" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="5" t="s">
+    <row r="103" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="6" t="s">
         <v>1128</v>
       </c>
-      <c r="B103" s="5" t="s">
+      <c r="B103" s="6" t="s">
         <v>1129</v>
       </c>
-      <c r="C103" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D103" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E103" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F103" s="5" t="s">
+      <c r="C103" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D103" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E103" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F103" s="6" t="s">
         <v>1240</v>
       </c>
-      <c r="H103" s="5" t="s">
+      <c r="H103" s="6" t="s">
         <v>1241</v>
       </c>
-      <c r="I103" s="5" t="n">
+      <c r="I103" s="6" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="J103" s="5" t="s">
+      <c r="J103" s="6" t="s">
         <v>1129</v>
       </c>
-      <c r="K103" s="5" t="s">
+      <c r="K103" s="6" t="s">
         <v>1242</v>
       </c>
-      <c r="L103" s="5" t="s">
+      <c r="L103" s="6" t="s">
         <v>1133</v>
       </c>
     </row>
-    <row r="104" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="5" t="s">
+    <row r="104" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="6" t="s">
         <v>1134</v>
       </c>
-      <c r="B104" s="5" t="s">
+      <c r="B104" s="6" t="s">
         <v>1129</v>
       </c>
-      <c r="C104" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D104" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E104" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F104" s="5" t="s">
+      <c r="C104" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D104" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E104" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F104" s="6" t="s">
         <v>1243</v>
       </c>
-      <c r="H104" s="5" t="s">
+      <c r="H104" s="6" t="s">
         <v>1243</v>
       </c>
-      <c r="I104" s="5" t="n">
+      <c r="I104" s="6" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="J104" s="5" t="s">
+      <c r="J104" s="6" t="s">
         <v>1129</v>
       </c>
-      <c r="K104" s="5" t="s">
+      <c r="K104" s="6" t="s">
         <v>1244</v>
       </c>
-      <c r="L104" s="5" t="s">
+      <c r="L104" s="6" t="s">
         <v>1213</v>
       </c>
     </row>
-    <row r="105" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="5" t="s">
+    <row r="105" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="6" t="s">
         <v>1142</v>
       </c>
-      <c r="B105" s="5" t="s">
+      <c r="B105" s="6" t="s">
         <v>1129</v>
       </c>
-      <c r="C105" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D105" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E105" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F105" s="5" t="s">
+      <c r="C105" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D105" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E105" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F105" s="6" t="s">
         <v>1245</v>
       </c>
-      <c r="H105" s="5" t="s">
+      <c r="H105" s="6" t="s">
         <v>1246</v>
       </c>
-      <c r="I105" s="5" t="n">
+      <c r="I105" s="6" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="J105" s="5" t="s">
+      <c r="J105" s="6" t="s">
         <v>1129</v>
       </c>
-      <c r="K105" s="5" t="s">
+      <c r="K105" s="6" t="s">
         <v>1247</v>
       </c>
-      <c r="L105" s="5" t="s">
+      <c r="L105" s="6" t="s">
         <v>1133</v>
       </c>
     </row>
-    <row r="106" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="5" t="s">
+    <row r="106" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="6" t="s">
         <v>1148</v>
       </c>
-      <c r="B106" s="5" t="s">
+      <c r="B106" s="6" t="s">
         <v>1129</v>
       </c>
-      <c r="C106" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D106" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E106" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F106" s="5" t="s">
+      <c r="C106" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D106" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E106" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F106" s="6" t="s">
         <v>1248</v>
       </c>
-      <c r="H106" s="5" t="s">
+      <c r="H106" s="6" t="s">
         <v>1249</v>
       </c>
-      <c r="I106" s="5" t="n">
+      <c r="I106" s="6" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="J106" s="5" t="s">
+      <c r="J106" s="6" t="s">
         <v>1129</v>
       </c>
-      <c r="K106" s="5" t="s">
+      <c r="K106" s="6" t="s">
         <v>1250</v>
       </c>
-      <c r="L106" s="5" t="s">
+      <c r="L106" s="6" t="s">
         <v>1133</v>
       </c>
     </row>
-    <row r="107" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="5" t="s">
+    <row r="107" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="6" t="s">
         <v>1155</v>
       </c>
-      <c r="B107" s="5" t="s">
+      <c r="B107" s="6" t="s">
         <v>1129</v>
       </c>
-      <c r="C107" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D107" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E107" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F107" s="5" t="s">
+      <c r="C107" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D107" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E107" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F107" s="6" t="s">
         <v>1251</v>
       </c>
-      <c r="H107" s="5" t="s">
+      <c r="H107" s="6" t="s">
         <v>1251</v>
       </c>
-      <c r="I107" s="5" t="n">
+      <c r="I107" s="6" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="J107" s="5" t="s">
+      <c r="J107" s="6" t="s">
         <v>1129</v>
       </c>
-      <c r="K107" s="5" t="s">
+      <c r="K107" s="6" t="s">
         <v>1252</v>
       </c>
-      <c r="L107" s="5" t="s">
+      <c r="L107" s="6" t="s">
         <v>1213</v>
       </c>
     </row>
@@ -22021,39 +22025,39 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="109" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="5" t="s">
+    <row r="109" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="6" t="s">
         <v>1175</v>
       </c>
-      <c r="B109" s="5" t="s">
+      <c r="B109" s="6" t="s">
         <v>1129</v>
       </c>
-      <c r="C109" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D109" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E109" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F109" s="5" t="s">
+      <c r="C109" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D109" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E109" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F109" s="6" t="s">
         <v>940</v>
       </c>
-      <c r="H109" s="5" t="s">
+      <c r="H109" s="6" t="s">
         <v>940</v>
       </c>
-      <c r="I109" s="5" t="n">
+      <c r="I109" s="6" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="J109" s="5" t="s">
+      <c r="J109" s="6" t="s">
         <v>1129</v>
       </c>
-      <c r="K109" s="5" t="s">
+      <c r="K109" s="6" t="s">
         <v>1253</v>
       </c>
-      <c r="L109" s="5" t="s">
+      <c r="L109" s="6" t="s">
         <v>1213</v>
       </c>
     </row>
@@ -23007,123 +23011,123 @@
         <v>1492</v>
       </c>
     </row>
-    <row r="137" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="6" t="s">
+    <row r="137" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="7" t="s">
         <v>1330</v>
       </c>
-      <c r="B137" s="6" t="s">
+      <c r="B137" s="7" t="s">
         <v>985</v>
       </c>
-      <c r="C137" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D137" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E137" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F137" s="6" t="s">
+      <c r="C137" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D137" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E137" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F137" s="7" t="s">
         <v>775</v>
       </c>
-      <c r="H137" s="6" t="s">
+      <c r="H137" s="7" t="s">
         <v>1326</v>
       </c>
-      <c r="I137" s="6" t="n">
+      <c r="I137" s="7" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="J137" s="6" t="s">
+      <c r="J137" s="7" t="s">
         <v>1293</v>
       </c>
-      <c r="K137" s="6" t="s">
+      <c r="K137" s="7" t="s">
         <v>1327</v>
       </c>
-      <c r="L137" s="6" t="s">
+      <c r="L137" s="7" t="s">
         <v>1328</v>
       </c>
     </row>
-    <row r="138" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="6" t="s">
+    <row r="138" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="7" t="s">
         <v>1331</v>
       </c>
-      <c r="B138" s="6" t="s">
+      <c r="B138" s="7" t="s">
         <v>985</v>
       </c>
-      <c r="C138" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D138" s="6" t="n">
+      <c r="C138" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D138" s="7" t="n">
         <v>13</v>
       </c>
     </row>
-    <row r="139" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="6" t="s">
+    <row r="139" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="7" t="s">
         <v>1332</v>
       </c>
-      <c r="B139" s="6" t="s">
+      <c r="B139" s="7" t="s">
         <v>985</v>
       </c>
-      <c r="C139" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D139" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="6" t="s">
+      <c r="C139" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D139" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="7" t="s">
         <v>1333</v>
       </c>
-      <c r="B140" s="6" t="s">
+      <c r="B140" s="7" t="s">
         <v>985</v>
       </c>
-      <c r="C140" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D140" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="6" t="s">
+      <c r="C140" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D140" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="7" t="s">
         <v>1334</v>
       </c>
-      <c r="B141" s="6" t="s">
+      <c r="B141" s="7" t="s">
         <v>985</v>
       </c>
-      <c r="C141" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D141" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="6" t="s">
+      <c r="C141" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D141" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="7" t="s">
         <v>1335</v>
       </c>
-      <c r="B142" s="6" t="s">
+      <c r="B142" s="7" t="s">
         <v>985</v>
       </c>
-      <c r="C142" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D142" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="6" t="s">
+      <c r="C142" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D142" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="7" t="s">
         <v>1336</v>
       </c>
-      <c r="B143" s="6" t="s">
+      <c r="B143" s="7" t="s">
         <v>985</v>
       </c>
-      <c r="C143" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D143" s="6" t="n">
+      <c r="C143" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D143" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -23543,101 +23547,101 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="158" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="6" t="s">
+    <row r="158" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="7" t="s">
         <v>1330</v>
       </c>
-      <c r="B158" s="6" t="s">
+      <c r="B158" s="7" t="s">
         <v>985</v>
       </c>
-      <c r="C158" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D158" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="159" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="6" t="s">
+      <c r="C158" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D158" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="7" t="s">
         <v>1331</v>
       </c>
-      <c r="B159" s="6" t="s">
+      <c r="B159" s="7" t="s">
         <v>985</v>
       </c>
-      <c r="C159" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D159" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="160" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="6" t="s">
+      <c r="C159" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D159" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="7" t="s">
         <v>1332</v>
       </c>
-      <c r="B160" s="6" t="s">
+      <c r="B160" s="7" t="s">
         <v>985</v>
       </c>
-      <c r="C160" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D160" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="161" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="6" t="s">
+      <c r="C160" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D160" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="7" t="s">
         <v>1333</v>
       </c>
-      <c r="B161" s="6" t="s">
+      <c r="B161" s="7" t="s">
         <v>985</v>
       </c>
-      <c r="C161" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D161" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="162" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="6" t="s">
+      <c r="C161" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D161" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="7" t="s">
         <v>1334</v>
       </c>
-      <c r="B162" s="6" t="s">
+      <c r="B162" s="7" t="s">
         <v>985</v>
       </c>
-      <c r="C162" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D162" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="163" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="6" t="s">
+      <c r="C162" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D162" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="7" t="s">
         <v>1335</v>
       </c>
-      <c r="B163" s="6" t="s">
+      <c r="B163" s="7" t="s">
         <v>985</v>
       </c>
-      <c r="C163" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D163" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="164" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="6" t="s">
+      <c r="C163" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D163" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="7" t="s">
         <v>1336</v>
       </c>
-      <c r="B164" s="6" t="s">
+      <c r="B164" s="7" t="s">
         <v>985</v>
       </c>
-      <c r="C164" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D164" s="6" t="n">
+      <c r="C164" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D164" s="7" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>